<commit_message>
remove the target folders and code changes for the altered plos jornal web page metadata
</commit_message>
<xml_diff>
--- a/plosdata/src/main/resources/plos_articles.xlsx
+++ b/plosdata/src/main/resources/plos_articles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="410">
   <si>
     <t>PLOS articles citation</t>
   </si>
@@ -1221,45 +1221,6 @@
     <t>Dwayne A. Elias</t>
   </si>
   <si>
-    <t>Tong Yuan</t>
-  </si>
-  <si>
-    <t>Metapopulation Dynamics Enable Persistence of Influenza A, Including A/H5N1, in Poultry</t>
-  </si>
-  <si>
-    <t>Hosseini PR, Fuller T, Harrigan R, Zhao D, Arriola CS, et al. (2013) Metapopulation Dynamics Enable Persistence of Influenza A, Including A/H5N1, in Poultry. PLoS ONE 8(12): e80091. doi:10.1371/journal.pone.0080091</t>
-  </si>
-  <si>
-    <t>Parviez Rana Hosseini</t>
-  </si>
-  <si>
-    <t>Peter Daszak</t>
-  </si>
-  <si>
-    <t>Trevon Fuller</t>
-  </si>
-  <si>
-    <t>Ryan Harrigan</t>
-  </si>
-  <si>
-    <t>Tom B. Smith</t>
-  </si>
-  <si>
-    <t>Delong Zhao</t>
-  </si>
-  <si>
-    <t>Carmen Sofia Arriola</t>
-  </si>
-  <si>
-    <t>Armandoe Gonzalez</t>
-  </si>
-  <si>
-    <t>Matthew Joshua Miller</t>
-  </si>
-  <si>
-    <t>Jamie Holland Jones</t>
-  </si>
-  <si>
     <t>Published</t>
   </si>
   <si>
@@ -1270,12 +1231,6 @@
   </si>
   <si>
     <t>Biochemistry</t>
-  </si>
-  <si>
-    <t>Institute for Environmental Genomics, Botany</t>
-  </si>
-  <si>
-    <t>Botany and Microbiology, Center for Spatial Analysis</t>
   </si>
   <si>
     <t>Bioengineering Center and Chemical, Biological and Materials Engineering</t>
@@ -2590,10 +2545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F367"/>
+  <dimension ref="A1:F344"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="B360" sqref="B360"/>
+      <selection activeCell="A350" sqref="A350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2633,7 +2588,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="F3" s="20"/>
     </row>
@@ -5093,7 +5048,7 @@
         <v>266</v>
       </c>
       <c r="C208" s="11" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D208" s="11" t="s">
         <v>276</v>
@@ -5867,7 +5822,7 @@
         <v>335</v>
       </c>
       <c r="C281" s="22" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D281" s="22" t="s">
         <v>338</v>
@@ -5883,7 +5838,7 @@
         <v>336</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D282" s="3"/>
       <c r="E282" s="30"/>
@@ -5895,7 +5850,7 @@
         <v>337</v>
       </c>
       <c r="C283" s="18" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="D283" s="13"/>
       <c r="E283" s="29"/>
@@ -6033,7 +5988,7 @@
         <v>351</v>
       </c>
       <c r="C295" s="13" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="D295" s="13"/>
       <c r="E295" s="29"/>
@@ -6071,7 +6026,7 @@
         <v>357</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="D298" s="3"/>
       <c r="E298" s="30"/>
@@ -6115,7 +6070,7 @@
         <v>362</v>
       </c>
       <c r="C302" s="22" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="D302" s="22" t="s">
         <v>361</v>
@@ -6547,283 +6502,37 @@
       <c r="E342" s="30"/>
       <c r="F342" s="20"/>
     </row>
-    <row r="343" spans="1:6">
-      <c r="A343" s="14"/>
-      <c r="B343" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="C343" s="3"/>
-      <c r="D343" s="3"/>
-      <c r="E343" s="30"/>
-      <c r="F343" s="20"/>
-    </row>
-    <row r="344" spans="1:6">
-      <c r="A344" s="14"/>
-      <c r="B344" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C344" s="3"/>
-      <c r="D344" s="3"/>
-      <c r="E344" s="30"/>
-      <c r="F344" s="20"/>
-    </row>
-    <row r="345" spans="1:6">
-      <c r="A345" s="14"/>
-      <c r="B345" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C345" s="3"/>
-      <c r="D345" s="3"/>
-      <c r="E345" s="30"/>
-      <c r="F345" s="20"/>
-    </row>
-    <row r="346" spans="1:6">
-      <c r="A346" s="14"/>
-      <c r="B346" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C346" s="3"/>
-      <c r="D346" s="3"/>
-      <c r="E346" s="30"/>
-      <c r="F346" s="20"/>
-    </row>
-    <row r="347" spans="1:6">
-      <c r="A347" s="14"/>
-      <c r="B347" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C347" s="3"/>
-      <c r="D347" s="3"/>
-      <c r="E347" s="30"/>
-      <c r="F347" s="20"/>
-    </row>
-    <row r="348" spans="1:6">
-      <c r="A348" s="14"/>
-      <c r="B348" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="C348" s="3"/>
-      <c r="D348" s="3"/>
-      <c r="E348" s="30"/>
-      <c r="F348" s="20"/>
-    </row>
-    <row r="349" spans="1:6">
-      <c r="A349" s="14"/>
-      <c r="B349" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C349" s="3"/>
-      <c r="D349" s="3"/>
-      <c r="E349" s="30"/>
-      <c r="F349" s="20"/>
-    </row>
-    <row r="350" spans="1:6">
-      <c r="A350" s="14"/>
-      <c r="B350" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C350" s="3"/>
-      <c r="D350" s="3"/>
-      <c r="E350" s="30"/>
-      <c r="F350" s="20"/>
-    </row>
-    <row r="351" spans="1:6">
-      <c r="A351" s="14"/>
-      <c r="B351" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C351" s="3"/>
-      <c r="D351" s="3"/>
-      <c r="E351" s="30"/>
-      <c r="F351" s="20"/>
-    </row>
-    <row r="352" spans="1:6">
-      <c r="A352" s="14"/>
-      <c r="B352" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="C352" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="D352" s="3"/>
-      <c r="E352" s="30"/>
-      <c r="F352" s="20"/>
-    </row>
-    <row r="353" spans="1:6">
-      <c r="A353" s="14"/>
-      <c r="B353" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C353" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="D353" s="3"/>
-      <c r="E353" s="30"/>
-      <c r="F353" s="20"/>
-    </row>
-    <row r="354" spans="1:6">
-      <c r="A354" s="12"/>
-      <c r="B354" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C354" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="D354" s="13"/>
-      <c r="E354" s="29"/>
-      <c r="F354" s="20"/>
-    </row>
-    <row r="355" spans="1:6" s="24" customFormat="1">
-      <c r="A355" s="36" t="s">
-        <v>401</v>
-      </c>
-      <c r="B355" s="22" t="s">
-        <v>403</v>
-      </c>
-      <c r="C355" s="22"/>
-      <c r="D355" s="22" t="s">
-        <v>402</v>
-      </c>
-      <c r="E355" s="37">
-        <v>41610</v>
-      </c>
-      <c r="F355" s="23"/>
-    </row>
-    <row r="356" spans="1:6">
-      <c r="A356" s="14"/>
-      <c r="B356" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="C356" s="3"/>
-      <c r="D356" s="3"/>
-      <c r="E356" s="30"/>
-      <c r="F356" s="20"/>
-    </row>
-    <row r="357" spans="1:6">
-      <c r="A357" s="14"/>
-      <c r="B357" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C357" s="3"/>
-      <c r="D357" s="3"/>
-      <c r="E357" s="30"/>
-      <c r="F357" s="20"/>
-    </row>
-    <row r="358" spans="1:6">
-      <c r="A358" s="14"/>
-      <c r="B358" s="3" t="s">
+    <row r="343" spans="1:6" ht="15" customHeight="1">
+      <c r="A343" s="41" t="s">
         <v>406</v>
       </c>
-      <c r="C358" s="3"/>
-      <c r="D358" s="3"/>
-      <c r="E358" s="30"/>
-      <c r="F358" s="20"/>
-    </row>
-    <row r="359" spans="1:6">
-      <c r="A359" s="14"/>
-      <c r="B359" s="3" t="s">
+      <c r="B343" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C343" s="41" t="s">
         <v>407</v>
       </c>
-      <c r="C359" s="3"/>
-      <c r="D359" s="3"/>
-      <c r="E359" s="30"/>
-      <c r="F359" s="20"/>
-    </row>
-    <row r="360" spans="1:6">
-      <c r="A360" s="14"/>
-      <c r="B360" s="3" t="s">
+      <c r="D343" s="41"/>
+      <c r="E343" s="42">
+        <v>38356</v>
+      </c>
+      <c r="F343"/>
+    </row>
+    <row r="344" spans="1:6" ht="15" customHeight="1">
+      <c r="A344" s="41"/>
+      <c r="B344" s="41" t="s">
         <v>408</v>
       </c>
-      <c r="C360" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D360" s="3"/>
-      <c r="E360" s="30"/>
-      <c r="F360" s="20"/>
-    </row>
-    <row r="361" spans="1:6">
-      <c r="A361" s="14"/>
-      <c r="B361" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C361" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D361" s="3"/>
-      <c r="E361" s="30"/>
-      <c r="F361" s="20"/>
-    </row>
-    <row r="362" spans="1:6">
-      <c r="A362" s="14"/>
-      <c r="B362" s="3" t="s">
+      <c r="C344" s="41" t="s">
+        <v>407</v>
+      </c>
+      <c r="D344" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="C362" s="3"/>
-      <c r="D362" s="3"/>
-      <c r="E362" s="30"/>
-      <c r="F362" s="20"/>
-    </row>
-    <row r="363" spans="1:6">
-      <c r="A363" s="14"/>
-      <c r="B363" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="C363" s="3"/>
-      <c r="D363" s="3"/>
-      <c r="E363" s="30"/>
-      <c r="F363" s="20"/>
-    </row>
-    <row r="364" spans="1:6">
-      <c r="A364" s="14"/>
-      <c r="B364" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C364" s="3"/>
-      <c r="D364" s="3"/>
-      <c r="E364" s="30"/>
-      <c r="F364" s="20"/>
-    </row>
-    <row r="365" spans="1:6">
-      <c r="A365" s="12"/>
-      <c r="B365" s="13" t="s">
-        <v>412</v>
-      </c>
-      <c r="C365" s="13"/>
-      <c r="D365" s="13"/>
-      <c r="E365" s="29"/>
-      <c r="F365" s="20"/>
-    </row>
-    <row r="366" spans="1:6" ht="15" customHeight="1">
-      <c r="A366" s="41" t="s">
-        <v>421</v>
-      </c>
-      <c r="B366" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C366" s="41" t="s">
-        <v>422</v>
-      </c>
-      <c r="D366" s="41"/>
-      <c r="E366" s="42">
+      <c r="E344" s="42">
         <v>38356</v>
       </c>
-      <c r="F366"/>
-    </row>
-    <row r="367" spans="1:6" ht="15" customHeight="1">
-      <c r="A367" s="41"/>
-      <c r="B367" s="41" t="s">
-        <v>423</v>
-      </c>
-      <c r="C367" s="41" t="s">
-        <v>422</v>
-      </c>
-      <c r="D367" s="41" t="s">
-        <v>424</v>
-      </c>
-      <c r="E367" s="42">
-        <v>38356</v>
-      </c>
-      <c r="F367"/>
+      <c r="F344"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>